<commit_message>
Forgot to save, whoops
</commit_message>
<xml_diff>
--- a/pics1_labeling.xlsx
+++ b/pics1_labeling.xlsx
@@ -550,9 +550,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
added features for pics1, a quarterthrough adding labels for pics3
</commit_message>
<xml_diff>
--- a/pics1_labeling.xlsx
+++ b/pics1_labeling.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="75">
   <si>
     <t>Name</t>
   </si>
@@ -231,6 +231,24 @@
   </si>
   <si>
     <t>Portrait Background</t>
+  </si>
+  <si>
+    <t>Other Faces in Photo</t>
+  </si>
+  <si>
+    <t>Flags in Photo</t>
+  </si>
+  <si>
+    <t>Other People in Photo</t>
+  </si>
+  <si>
+    <t>Looking Left</t>
+  </si>
+  <si>
+    <t>Looking Center</t>
+  </si>
+  <si>
+    <t>Looking Right</t>
   </si>
 </sst>
 </file>
@@ -548,11 +566,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S25"/>
+  <dimension ref="A1:Y25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Y16" sqref="Y16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -566,7 +584,7 @@
     <col min="17" max="17" width="10.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -624,8 +642,26 @@
       <c r="S1" t="s">
         <v>68</v>
       </c>
+      <c r="T1" t="s">
+        <v>71</v>
+      </c>
+      <c r="U1" t="s">
+        <v>69</v>
+      </c>
+      <c r="V1" t="s">
+        <v>70</v>
+      </c>
+      <c r="W1" t="s">
+        <v>72</v>
+      </c>
+      <c r="X1" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>74</v>
+      </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -683,8 +719,26 @@
       <c r="S2" t="s">
         <v>66</v>
       </c>
+      <c r="T2" t="s">
+        <v>67</v>
+      </c>
+      <c r="U2" t="s">
+        <v>67</v>
+      </c>
+      <c r="V2" t="s">
+        <v>67</v>
+      </c>
+      <c r="W2" t="s">
+        <v>67</v>
+      </c>
+      <c r="X2" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -742,8 +796,26 @@
       <c r="S3" t="s">
         <v>67</v>
       </c>
+      <c r="T3" t="s">
+        <v>67</v>
+      </c>
+      <c r="U3" t="s">
+        <v>67</v>
+      </c>
+      <c r="V3" t="s">
+        <v>67</v>
+      </c>
+      <c r="W3" t="s">
+        <v>67</v>
+      </c>
+      <c r="X3" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -801,8 +873,26 @@
       <c r="S4" t="s">
         <v>66</v>
       </c>
+      <c r="T4" t="s">
+        <v>67</v>
+      </c>
+      <c r="U4" t="s">
+        <v>67</v>
+      </c>
+      <c r="V4" t="s">
+        <v>67</v>
+      </c>
+      <c r="W4" t="s">
+        <v>67</v>
+      </c>
+      <c r="X4" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -860,8 +950,26 @@
       <c r="S5" t="s">
         <v>67</v>
       </c>
+      <c r="T5" t="s">
+        <v>67</v>
+      </c>
+      <c r="U5" t="s">
+        <v>67</v>
+      </c>
+      <c r="V5" t="s">
+        <v>67</v>
+      </c>
+      <c r="W5" t="s">
+        <v>67</v>
+      </c>
+      <c r="X5" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -919,8 +1027,26 @@
       <c r="S6" t="s">
         <v>67</v>
       </c>
+      <c r="T6" t="s">
+        <v>67</v>
+      </c>
+      <c r="U6" t="s">
+        <v>67</v>
+      </c>
+      <c r="V6" t="s">
+        <v>67</v>
+      </c>
+      <c r="W6" t="s">
+        <v>67</v>
+      </c>
+      <c r="X6" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -978,8 +1104,26 @@
       <c r="S7" t="s">
         <v>67</v>
       </c>
+      <c r="T7" t="s">
+        <v>67</v>
+      </c>
+      <c r="U7" t="s">
+        <v>67</v>
+      </c>
+      <c r="V7" t="s">
+        <v>67</v>
+      </c>
+      <c r="W7" t="s">
+        <v>67</v>
+      </c>
+      <c r="X7" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1037,8 +1181,26 @@
       <c r="S8" t="s">
         <v>66</v>
       </c>
+      <c r="T8" t="s">
+        <v>67</v>
+      </c>
+      <c r="U8" t="s">
+        <v>67</v>
+      </c>
+      <c r="V8" t="s">
+        <v>67</v>
+      </c>
+      <c r="W8" t="s">
+        <v>67</v>
+      </c>
+      <c r="X8" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1096,8 +1258,26 @@
       <c r="S9" t="s">
         <v>66</v>
       </c>
+      <c r="T9" t="s">
+        <v>67</v>
+      </c>
+      <c r="U9" t="s">
+        <v>67</v>
+      </c>
+      <c r="V9" t="s">
+        <v>67</v>
+      </c>
+      <c r="W9" t="s">
+        <v>67</v>
+      </c>
+      <c r="X9" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -1155,8 +1335,26 @@
       <c r="S10" t="s">
         <v>67</v>
       </c>
+      <c r="T10" t="s">
+        <v>67</v>
+      </c>
+      <c r="U10" t="s">
+        <v>67</v>
+      </c>
+      <c r="V10" t="s">
+        <v>67</v>
+      </c>
+      <c r="W10" t="s">
+        <v>67</v>
+      </c>
+      <c r="X10" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -1214,8 +1412,26 @@
       <c r="S11" t="s">
         <v>66</v>
       </c>
+      <c r="T11" t="s">
+        <v>67</v>
+      </c>
+      <c r="U11" t="s">
+        <v>67</v>
+      </c>
+      <c r="V11" t="s">
+        <v>67</v>
+      </c>
+      <c r="W11" t="s">
+        <v>67</v>
+      </c>
+      <c r="X11" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1273,8 +1489,26 @@
       <c r="S12" t="s">
         <v>66</v>
       </c>
+      <c r="T12" t="s">
+        <v>67</v>
+      </c>
+      <c r="U12" t="s">
+        <v>67</v>
+      </c>
+      <c r="V12" t="s">
+        <v>67</v>
+      </c>
+      <c r="W12" t="s">
+        <v>67</v>
+      </c>
+      <c r="X12" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -1332,8 +1566,26 @@
       <c r="S13" t="s">
         <v>67</v>
       </c>
+      <c r="T13" t="s">
+        <v>67</v>
+      </c>
+      <c r="U13" t="s">
+        <v>67</v>
+      </c>
+      <c r="V13" t="s">
+        <v>67</v>
+      </c>
+      <c r="W13" t="s">
+        <v>67</v>
+      </c>
+      <c r="X13" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1391,8 +1643,26 @@
       <c r="S14" t="s">
         <v>67</v>
       </c>
+      <c r="T14" t="s">
+        <v>67</v>
+      </c>
+      <c r="U14" t="s">
+        <v>67</v>
+      </c>
+      <c r="V14" t="s">
+        <v>67</v>
+      </c>
+      <c r="W14" t="s">
+        <v>67</v>
+      </c>
+      <c r="X14" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -1450,8 +1720,26 @@
       <c r="S15" t="s">
         <v>67</v>
       </c>
+      <c r="T15" t="s">
+        <v>67</v>
+      </c>
+      <c r="U15" t="s">
+        <v>67</v>
+      </c>
+      <c r="V15" t="s">
+        <v>67</v>
+      </c>
+      <c r="W15" t="s">
+        <v>67</v>
+      </c>
+      <c r="X15" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -1509,8 +1797,26 @@
       <c r="S16" t="s">
         <v>67</v>
       </c>
+      <c r="T16" t="s">
+        <v>67</v>
+      </c>
+      <c r="U16" t="s">
+        <v>67</v>
+      </c>
+      <c r="V16" t="s">
+        <v>67</v>
+      </c>
+      <c r="W16" t="s">
+        <v>67</v>
+      </c>
+      <c r="X16" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -1568,8 +1874,26 @@
       <c r="S17" t="s">
         <v>66</v>
       </c>
+      <c r="T17" t="s">
+        <v>67</v>
+      </c>
+      <c r="U17" t="s">
+        <v>67</v>
+      </c>
+      <c r="V17" t="s">
+        <v>67</v>
+      </c>
+      <c r="W17" t="s">
+        <v>67</v>
+      </c>
+      <c r="X17" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -1627,8 +1951,26 @@
       <c r="S18" t="s">
         <v>67</v>
       </c>
+      <c r="T18" t="s">
+        <v>67</v>
+      </c>
+      <c r="U18" t="s">
+        <v>67</v>
+      </c>
+      <c r="V18" t="s">
+        <v>67</v>
+      </c>
+      <c r="W18" t="s">
+        <v>67</v>
+      </c>
+      <c r="X18" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -1686,8 +2028,26 @@
       <c r="S19" t="s">
         <v>67</v>
       </c>
+      <c r="T19" t="s">
+        <v>67</v>
+      </c>
+      <c r="U19" t="s">
+        <v>67</v>
+      </c>
+      <c r="V19" t="s">
+        <v>67</v>
+      </c>
+      <c r="W19" t="s">
+        <v>67</v>
+      </c>
+      <c r="X19" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -1745,8 +2105,26 @@
       <c r="S20" t="s">
         <v>67</v>
       </c>
+      <c r="T20" t="s">
+        <v>67</v>
+      </c>
+      <c r="U20" t="s">
+        <v>67</v>
+      </c>
+      <c r="V20" t="s">
+        <v>67</v>
+      </c>
+      <c r="W20" t="s">
+        <v>67</v>
+      </c>
+      <c r="X20" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -1804,8 +2182,26 @@
       <c r="S21" t="s">
         <v>67</v>
       </c>
+      <c r="T21" t="s">
+        <v>67</v>
+      </c>
+      <c r="U21" t="s">
+        <v>67</v>
+      </c>
+      <c r="V21" t="s">
+        <v>67</v>
+      </c>
+      <c r="W21" t="s">
+        <v>67</v>
+      </c>
+      <c r="X21" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -1863,8 +2259,26 @@
       <c r="S22" t="s">
         <v>66</v>
       </c>
+      <c r="T22" t="s">
+        <v>67</v>
+      </c>
+      <c r="U22" t="s">
+        <v>67</v>
+      </c>
+      <c r="V22" t="s">
+        <v>67</v>
+      </c>
+      <c r="W22" t="s">
+        <v>67</v>
+      </c>
+      <c r="X22" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>44</v>
       </c>
@@ -1922,8 +2336,26 @@
       <c r="S23" t="s">
         <v>67</v>
       </c>
+      <c r="T23" t="s">
+        <v>67</v>
+      </c>
+      <c r="U23" t="s">
+        <v>67</v>
+      </c>
+      <c r="V23" t="s">
+        <v>67</v>
+      </c>
+      <c r="W23" t="s">
+        <v>67</v>
+      </c>
+      <c r="X23" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>46</v>
       </c>
@@ -1981,8 +2413,26 @@
       <c r="S24" t="s">
         <v>67</v>
       </c>
+      <c r="T24" t="s">
+        <v>67</v>
+      </c>
+      <c r="U24" t="s">
+        <v>67</v>
+      </c>
+      <c r="V24" t="s">
+        <v>67</v>
+      </c>
+      <c r="W24" t="s">
+        <v>67</v>
+      </c>
+      <c r="X24" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>48</v>
       </c>
@@ -2038,6 +2488,24 @@
         <v>66</v>
       </c>
       <c r="S25" t="s">
+        <v>67</v>
+      </c>
+      <c r="T25" t="s">
+        <v>67</v>
+      </c>
+      <c r="U25" t="s">
+        <v>67</v>
+      </c>
+      <c r="V25" t="s">
+        <v>67</v>
+      </c>
+      <c r="W25" t="s">
+        <v>67</v>
+      </c>
+      <c r="X25" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y25" t="s">
         <v>67</v>
       </c>
     </row>

</xml_diff>